<commit_message>
rat la quan trong #ca
</commit_message>
<xml_diff>
--- a/File/SubSheet.xlsx
+++ b/File/SubSheet.xlsx
@@ -25,12 +25,6 @@
     <x:t>From</x:t>
   </x:si>
   <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mail</x:t>
-  </x:si>
-  <x:si>
     <x:t>Subject</x:t>
   </x:si>
   <x:si>
@@ -43,16 +37,37 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
+    <x:t>Sat, 26 Oct 2024 04:26:02 +0000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>"Google" &lt;no-reply@accounts.google.com&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Security alert</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">[image: Google]
+App password created to sign in to your account
+nennhayen@gmail.com
+If you didn't generate this password for Sendmail, someone might be using
+your account. Check and secure your account now.
+Check activity
+&lt;https://accounts.google.com/AccountChooser?Email=nennhayen@gmail.com&amp;continue=https://myaccount.google.com/alert/nt/1729916762411?rfn%3D20%26rfnc%3D1%26eid%3D2585404366186269778%26et%3D0&gt;
+You can also see security activity at
+https://myaccount.google.com/notifications
+You received this email to let you know about important changes to your
+Google Account and services.
+© 2024 Google LLC, 1600 Amphitheatre Parkway, Mountain View, CA 94043, USA
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sat, 26 Oct 2024 11:03:11 +0700</x:t>
   </x:si>
   <x:si>
     <x:t>"Nguyễn Thị Mai Bình" &lt;maibinh6223@gmail.com&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Thị Mai Bình</x:t>
-  </x:si>
-  <x:si>
-    <x:t>maibinh6223@gmail.com</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Kính gửi bộ phận hỗ trợ,
@@ -79,19 +94,13 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
+    <x:t>3</x:t>
   </x:si>
   <x:si>
     <x:t>Sun, 20 Oct 2024 13:37:30 +0000</x:t>
   </x:si>
   <x:si>
     <x:t>"Thùy Dung Trần" &lt;thuydungtran018@gmail.com&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thùy Dung Trần</x:t>
-  </x:si>
-  <x:si>
-    <x:t>thuydungtran018@gmail.com</x:t>
   </x:si>
   <x:si>
     <x:t>Yêu cầu hỗ trợ về sản phẩm Máy Rửa Chén Bát Độc Lập Bosch 13 bộ SMS4EKI06E- Series 4, màu inox bạc</x:t>
@@ -111,7 +120,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
+    <x:t>4</x:t>
   </x:si>
   <x:si>
     <x:t>Sun, 20 Oct 2024 13:42:48 +0000</x:t>
@@ -131,22 +140,10 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
+    <x:t>5</x:t>
   </x:si>
   <x:si>
     <x:t>Sun, 20 Oct 2024 13:14:29 +0000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>"Google" &lt;no-reply@accounts.google.com&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Google</x:t>
-  </x:si>
-  <x:si>
-    <x:t>no-reply@accounts.google.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Security alert</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">[image: Google]
@@ -162,42 +159,6 @@
 Google Account and services.
 © 2024 Google LLC, 1600 Amphitheatre Parkway, Mountain View, CA 94043, USA
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thu, 24 Oct 2024 16:01:43 +0800</x:t>
-  </x:si>
-  <x:si>
-    <x:t>"Lazada Vietnam" &lt;noreply@support.lazada.vn&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>"Lazada Vietnam"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>noreply@support.lazada.vn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Policy: Inactive seller (Holiday Mode)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;p id="u9951d5f7"&gt; &lt;/p&gt;
-&lt;p id="u5baee0d4"&gt;&lt;img id="ed7lA" src="https://intranetproxy.alipay.com/skylark/lark/0/2022/png/48956351/1669201155248-42ab56dc-aa34-41c5-b03d-2ff702ab448e.png" width="940" /&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Thân gửi &lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;Nến Nhà Yên ( VN345D0BTN ),&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Đã hơn 89 ngày bạn không đăng nhập vào gian hàng của mình?&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Để giúp duy trì sự cạnh tranh với các gian hàng khác đồng thời đảm bảo việc xử lý đơn hàng, phản hồi người mua kịp thời, Lazada khuyến khích bạn đăng nhập vào gian hàng thường xuyên để cập nhật hàng tồn kho, khuyến mãi và giá bán mới.&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Nhằm đảm bảo trải nghiệm của người mua, gian hàng của bạn có thể sẽ tự động bật &lt;b&gt;"Chế độ nghỉ lễ"&lt;/b&gt; nếu tiếp tục không đăng nhập vào gian hàng. Tìm hiểu thêm thông tin [&lt;/span&gt;&lt;/span&gt;&lt;a href="https://sellercenter.lazada.vn/seller/helpcenter/chinh-sach-ve-nha-ban-hang-khong-hoat-dong-8176.html" style="color:blue; text-decoration:underline"&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;tại đây&lt;/span&gt;&lt;/span&gt;&lt;/a&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;]&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Cảm ơn sự hợp tác của bạn&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Đội ngũ Lazada Việt Nam&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;hr id="gD6cB" /&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Dear &lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;Nến Nhà Yên ( VN345D0BTN ),&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Our records show that your seller account has been inactive for &lt;b&gt;over 89 days&lt;/b&gt; and we kindly request that you log in regularly to update your inventory, promotions and prices. This will help you maintain the competitiveness of your listings within our platform.&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;To ensure that your buyers' experience is not compromised, your seller account may have &lt;/span&gt;&lt;/span&gt;&lt;a href="https://sellercenter.lazada.vn/seller/helpcenter/chinh-sach-ve-nha-ban-hang-khong-hoat-dong-8176.html" style="color:blue; text-decoration:underline" target="_blank"&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Holiday Mode&lt;/span&gt;&lt;/span&gt;&lt;/a&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt; turned on by next week if it continues to be inactive. We urge you to take action and keep your account active now. Click &lt;/span&gt;&lt;/span&gt;&lt;a href="https://sellercenter.lazada.vn/seller/helpcenter/chinh-sach-ve-nha-ban-hang-khong-hoat-dong-8176.html" style="color:blue; text-decoration:underline" target="_blank"&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;here&lt;/span&gt;&lt;/span&gt;&lt;/a&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt; to learn more.&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Thank you.&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-size:12pt"&gt;&lt;span new="" roman="" style="font-family:" times=""&gt;&lt;span style="font-size:10.0pt"&gt;&lt;span calibri="" style="font-family:"&gt;Best regards, &lt;br /&gt;
-Lazada Vietnam&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;div style="display:none"&gt;&lt;img style="display:none" src="http://gm.mmstat.com/global-message-platform-ae.edm.edm_open?site_id=VN&amp;t=1729756903362&amp;msg_id=91281fd3-08bc-4b8c-822a-345e00643473&amp;template_name=Policy_Inactive Seller T-1_Notification-0_VN&amp;to_address=nennhayen@gmail.com"/&gt;&lt;/div&gt;&lt;div style="display:none"&gt;&lt;img style="display:none" src="https://sg.mmstat.com/lzdseller.email-engagement.api-tracking?gmkey=EXP&amp;gokey=site_id%3DVN%26t%3D1729756903362%26msg_id%3D91281fd3-08bc-4b8c-822a-345e00643473%26mq_msg_id%3D21016D63588A609E076579E2BF8B79B6%26to_address%3Dnennhayen%40gmail.com%26requirement_id%3D489%26template_id%3D4540%26template_name%3DPolicy_Inactive+Seller+T-1_Notification-0_VN&amp;logtype=2"/&gt;&lt;/div&gt;</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -552,13 +513,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H2"/>
+  <x:dimension ref="A1:F2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -577,123 +538,87 @@
       <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" s="0" t="s">
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G2" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G3" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G4" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="G5" s="1" t="s">
-        <x:v>31</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="G6" s="1" t="s">
-        <x:v>38</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>